<commit_message>
final analysis by toshi
</commit_message>
<xml_diff>
--- a/analysis/20(vs20-40).xlsx
+++ b/analysis/20(vs20-40).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshi A. Furukawa\Dropbox\AAAAA\SYSTEMATIC REVIEWS\2017-06-30 GRISELDA\2019-06-XX fixed vs flexible regimens\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tshkf\Dropbox\AAAAA\SYSTEMATIC REVIEWS\2017-06-30 GRISELDA\2019-10-27 fixed vs flexible regimens\analysis2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56858E0-50CC-4DFD-BDAD-FF603B136252}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D13937F-7D88-43ED-A63A-FE2826EADEFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{B2778113-3313-46F3-9886-20FA084463AB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="166">
   <si>
     <t>StudyID</t>
   </si>
@@ -512,13 +512,37 @@
   </si>
   <si>
     <t>SSRI</t>
+  </si>
+  <si>
+    <t>paroxetine</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Trivedi2004 (29060/810) CR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Unclear</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Moderate risk</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rapaport2009 (BRL-29060/874) (NCT00067444) CR</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,16 +571,29 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -564,13 +601,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -578,8 +633,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="メモ" xfId="1" builtinId="10"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -892,13 +951,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E8ECBC-DD29-46BA-A49A-044BF3258F7B}">
-  <dimension ref="A1:AU64"/>
+  <dimension ref="A1:AU68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK34" workbookViewId="0">
-      <selection activeCell="AT34" sqref="AT1:AT1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G35" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="25.08203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
@@ -1379,16 +1444,16 @@
         <v>28</v>
       </c>
       <c r="Q4">
-        <v>105</v>
+        <v>52.5</v>
       </c>
       <c r="R4">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>101</v>
+        <v>50.5</v>
       </c>
       <c r="U4">
         <v>-12.1</v>
@@ -1397,10 +1462,10 @@
         <v>11.05</v>
       </c>
       <c r="W4">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="X4">
-        <v>19</v>
+        <v>9.5</v>
       </c>
       <c r="Y4" t="s">
         <v>48</v>
@@ -8624,13 +8689,13 @@
     </row>
     <row r="55" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B55">
-        <v>2012</v>
+        <v>2001</v>
       </c>
       <c r="C55">
-        <v>43.7</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="D55" t="s">
         <v>70</v>
@@ -8639,70 +8704,70 @@
         <v>157</v>
       </c>
       <c r="F55" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="G55">
         <v>6</v>
       </c>
       <c r="H55">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I55">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="J55">
-        <v>6</v>
-      </c>
-      <c r="K55" t="s">
-        <v>70</v>
+        <v>23</v>
+      </c>
+      <c r="K55">
+        <v>9</v>
       </c>
       <c r="L55">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="M55">
-        <v>21.67</v>
+        <v>-13.8</v>
       </c>
       <c r="N55">
-        <v>13.14</v>
+        <v>10.83</v>
       </c>
       <c r="O55">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="P55">
+        <v>23</v>
+      </c>
+      <c r="Q55">
+        <v>52.5</v>
+      </c>
+      <c r="R55">
         <v>9</v>
       </c>
-      <c r="Q55">
-        <v>30</v>
-      </c>
-      <c r="R55">
-        <v>4</v>
-      </c>
-      <c r="S55" t="s">
-        <v>70</v>
+      <c r="S55">
+        <v>1</v>
       </c>
       <c r="T55">
-        <v>30</v>
+        <v>50.5</v>
       </c>
       <c r="U55">
-        <v>24.73</v>
+        <v>-12.1</v>
       </c>
       <c r="V55">
-        <v>8.65</v>
+        <v>11.05</v>
       </c>
       <c r="W55">
+        <v>18</v>
+      </c>
+      <c r="X55">
+        <v>9.5</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z55">
         <v>5</v>
       </c>
-      <c r="X55">
-        <v>4</v>
-      </c>
-      <c r="Y55" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z55">
-        <v>4</v>
-      </c>
       <c r="AA55" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="AB55" t="s">
         <v>50</v>
@@ -8711,10 +8776,10 @@
         <v>51</v>
       </c>
       <c r="AD55" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="AE55" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="AF55" t="s">
         <v>54</v>
@@ -8723,10 +8788,10 @@
         <v>80</v>
       </c>
       <c r="AH55" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI55">
-        <v>17</v>
+        <v>75</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>70</v>
       </c>
       <c r="AJ55" t="s">
         <v>57</v>
@@ -8735,114 +8800,114 @@
         <v>6</v>
       </c>
       <c r="AL55" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="AM55" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN55" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO55" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP55" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ55" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR55" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS55" t="s">
         <v>58</v>
       </c>
-      <c r="AN55" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO55" t="s">
-        <v>58</v>
-      </c>
-      <c r="AP55" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ55" t="s">
-        <v>60</v>
-      </c>
-      <c r="AR55" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS55" t="s">
-        <v>60</v>
-      </c>
       <c r="AT55" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="AU55" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>142</v>
-      </c>
-      <c r="B56" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56" t="s">
-        <v>70</v>
+        <v>161</v>
+      </c>
+      <c r="B56">
+        <v>2004</v>
+      </c>
+      <c r="C56">
+        <v>39.4</v>
       </c>
       <c r="D56" t="s">
-        <v>70</v>
+        <v>162</v>
       </c>
       <c r="E56" t="s">
         <v>157</v>
       </c>
       <c r="F56" t="s">
-        <v>141</v>
-      </c>
-      <c r="G56" t="s">
-        <v>70</v>
+        <v>160</v>
+      </c>
+      <c r="G56">
+        <v>8</v>
       </c>
       <c r="H56">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I56">
-        <v>26</v>
+        <v>154</v>
       </c>
       <c r="J56">
-        <v>9</v>
-      </c>
-      <c r="K56" t="s">
-        <v>70</v>
-      </c>
-      <c r="L56" t="s">
-        <v>70</v>
-      </c>
-      <c r="M56" t="s">
-        <v>70</v>
-      </c>
-      <c r="N56" t="s">
-        <v>70</v>
-      </c>
-      <c r="O56" t="s">
-        <v>70</v>
-      </c>
-      <c r="P56" t="s">
-        <v>70</v>
+        <v>44</v>
+      </c>
+      <c r="K56">
+        <v>10</v>
+      </c>
+      <c r="L56">
+        <v>143</v>
+      </c>
+      <c r="M56">
+        <v>-12.4</v>
+      </c>
+      <c r="N56">
+        <v>7.1749000000000001</v>
+      </c>
+      <c r="O56">
+        <v>91</v>
+      </c>
+      <c r="P56">
+        <v>58</v>
       </c>
       <c r="Q56">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="R56">
-        <v>8</v>
-      </c>
-      <c r="S56" t="s">
-        <v>70</v>
-      </c>
-      <c r="T56" t="s">
-        <v>70</v>
-      </c>
-      <c r="U56" t="s">
-        <v>70</v>
-      </c>
-      <c r="V56" t="s">
-        <v>70</v>
-      </c>
-      <c r="W56" t="s">
-        <v>70</v>
-      </c>
-      <c r="X56" t="s">
-        <v>70</v>
+        <v>36</v>
+      </c>
+      <c r="S56">
+        <v>6</v>
+      </c>
+      <c r="T56">
+        <v>142</v>
+      </c>
+      <c r="U56">
+        <v>-10</v>
+      </c>
+      <c r="V56">
+        <v>7.149</v>
+      </c>
+      <c r="W56">
+        <v>72</v>
+      </c>
+      <c r="X56">
+        <v>37</v>
       </c>
       <c r="Y56" t="s">
         <v>48</v>
       </c>
       <c r="Z56">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AA56" t="s">
         <v>79</v>
@@ -8857,25 +8922,25 @@
         <v>52</v>
       </c>
       <c r="AE56" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="AF56" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="AG56" t="s">
-        <v>143</v>
+        <v>71</v>
       </c>
       <c r="AH56" t="s">
         <v>56</v>
       </c>
       <c r="AI56">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AJ56" t="s">
         <v>48</v>
       </c>
       <c r="AK56">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AL56" t="s">
         <v>86</v>
@@ -8896,96 +8961,96 @@
         <v>60</v>
       </c>
       <c r="AR56" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AS56" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="AT56" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="AU56" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>144</v>
-      </c>
-      <c r="B57" t="s">
-        <v>70</v>
+        <v>165</v>
+      </c>
+      <c r="B57">
+        <v>2009</v>
       </c>
       <c r="C57">
-        <v>37</v>
-      </c>
-      <c r="D57">
-        <v>0.47241149999999998</v>
+        <v>67</v>
+      </c>
+      <c r="D57" t="s">
+        <v>162</v>
       </c>
       <c r="E57" t="s">
         <v>157</v>
       </c>
       <c r="F57" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="G57">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H57">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I57">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="J57">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K57">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L57">
-        <v>90</v>
+        <v>173</v>
       </c>
       <c r="M57">
-        <v>-10.6</v>
+        <v>-12.11</v>
       </c>
       <c r="N57">
-        <v>8.6</v>
+        <v>7.9960000000000004</v>
       </c>
       <c r="O57">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="P57">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="Q57">
-        <v>91</v>
+        <v>180</v>
       </c>
       <c r="R57">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="S57">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="T57">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="U57">
-        <v>-7.6</v>
+        <v>-8.85</v>
       </c>
       <c r="V57">
-        <v>7.5</v>
+        <v>8.0449999999999999</v>
       </c>
       <c r="W57">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="X57">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="Y57" t="s">
         <v>48</v>
       </c>
       <c r="Z57">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA57" t="s">
         <v>79</v>
@@ -9003,7 +9068,7 @@
         <v>71</v>
       </c>
       <c r="AF57" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="AG57" t="s">
         <v>80</v>
@@ -9012,19 +9077,19 @@
         <v>56</v>
       </c>
       <c r="AI57">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AJ57" t="s">
         <v>48</v>
       </c>
       <c r="AK57">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AL57" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="AM57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AN57" t="s">
         <v>60</v>
@@ -9045,21 +9110,21 @@
         <v>58</v>
       </c>
       <c r="AT57" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="AU57" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>145</v>
-      </c>
-      <c r="B58" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" t="s">
-        <v>70</v>
+        <v>140</v>
+      </c>
+      <c r="B58">
+        <v>2012</v>
+      </c>
+      <c r="C58">
+        <v>43.7</v>
       </c>
       <c r="D58" t="s">
         <v>70</v>
@@ -9070,68 +9135,68 @@
       <c r="F58" t="s">
         <v>141</v>
       </c>
-      <c r="G58" t="s">
-        <v>70</v>
+      <c r="G58">
+        <v>6</v>
       </c>
       <c r="H58">
         <v>50</v>
       </c>
       <c r="I58">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J58">
+        <v>6</v>
+      </c>
+      <c r="K58" t="s">
+        <v>70</v>
+      </c>
+      <c r="L58">
+        <v>30</v>
+      </c>
+      <c r="M58">
+        <v>21.67</v>
+      </c>
+      <c r="N58">
+        <v>13.14</v>
+      </c>
+      <c r="O58">
         <v>10</v>
       </c>
-      <c r="K58" t="s">
-        <v>70</v>
-      </c>
-      <c r="L58" t="s">
-        <v>70</v>
-      </c>
-      <c r="M58" t="s">
-        <v>70</v>
-      </c>
-      <c r="N58" t="s">
-        <v>70</v>
-      </c>
-      <c r="O58" t="s">
-        <v>70</v>
-      </c>
-      <c r="P58" t="s">
-        <v>70</v>
+      <c r="P58">
+        <v>9</v>
       </c>
       <c r="Q58">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="R58">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="S58" t="s">
         <v>70</v>
       </c>
-      <c r="T58" t="s">
-        <v>70</v>
-      </c>
-      <c r="U58" t="s">
-        <v>70</v>
-      </c>
-      <c r="V58" t="s">
-        <v>70</v>
-      </c>
-      <c r="W58" t="s">
-        <v>70</v>
-      </c>
-      <c r="X58" t="s">
-        <v>70</v>
+      <c r="T58">
+        <v>30</v>
+      </c>
+      <c r="U58">
+        <v>24.73</v>
+      </c>
+      <c r="V58">
+        <v>8.65</v>
+      </c>
+      <c r="W58">
+        <v>5</v>
+      </c>
+      <c r="X58">
+        <v>4</v>
       </c>
       <c r="Y58" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="Z58">
         <v>4</v>
       </c>
       <c r="AA58" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="AB58" t="s">
         <v>50</v>
@@ -9140,40 +9205,40 @@
         <v>51</v>
       </c>
       <c r="AD58" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="AE58" t="s">
         <v>85</v>
       </c>
       <c r="AF58" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="AG58" t="s">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="AH58" t="s">
         <v>56</v>
       </c>
       <c r="AI58">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AJ58" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AK58">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AL58" t="s">
         <v>48</v>
       </c>
       <c r="AM58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AN58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AO58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AP58" t="s">
         <v>59</v>
@@ -9182,96 +9247,96 @@
         <v>60</v>
       </c>
       <c r="AR58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AS58" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="AT58" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="AU58" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>149</v>
-      </c>
-      <c r="B59">
-        <v>1998</v>
-      </c>
-      <c r="C59">
-        <v>41.75</v>
-      </c>
-      <c r="D59">
-        <v>0.64500000000000002</v>
+        <v>142</v>
+      </c>
+      <c r="B59" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" t="s">
+        <v>70</v>
       </c>
       <c r="E59" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F59" t="s">
-        <v>147</v>
-      </c>
-      <c r="G59">
+        <v>141</v>
+      </c>
+      <c r="G59" t="s">
+        <v>70</v>
+      </c>
+      <c r="H59">
+        <v>50</v>
+      </c>
+      <c r="I59">
+        <v>26</v>
+      </c>
+      <c r="J59">
+        <v>9</v>
+      </c>
+      <c r="K59" t="s">
+        <v>70</v>
+      </c>
+      <c r="L59" t="s">
+        <v>70</v>
+      </c>
+      <c r="M59" t="s">
+        <v>70</v>
+      </c>
+      <c r="N59" t="s">
+        <v>70</v>
+      </c>
+      <c r="O59" t="s">
+        <v>70</v>
+      </c>
+      <c r="P59" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q59">
+        <v>26</v>
+      </c>
+      <c r="R59">
         <v>8</v>
       </c>
-      <c r="H59">
-        <v>75</v>
-      </c>
-      <c r="I59">
-        <v>85</v>
-      </c>
-      <c r="J59" t="s">
-        <v>70</v>
-      </c>
-      <c r="K59">
-        <v>24</v>
-      </c>
-      <c r="L59">
-        <v>83</v>
-      </c>
-      <c r="M59">
-        <v>13.69</v>
-      </c>
-      <c r="N59">
-        <v>7.47</v>
-      </c>
-      <c r="O59">
-        <v>42</v>
-      </c>
-      <c r="P59">
-        <v>19</v>
-      </c>
-      <c r="Q59">
-        <v>95</v>
-      </c>
-      <c r="R59" t="s">
-        <v>70</v>
-      </c>
-      <c r="S59">
-        <v>6</v>
-      </c>
-      <c r="T59">
-        <v>93</v>
-      </c>
-      <c r="U59">
-        <v>17.25</v>
-      </c>
-      <c r="V59">
-        <v>7.43</v>
-      </c>
-      <c r="W59">
-        <v>32</v>
-      </c>
-      <c r="X59">
-        <v>10</v>
+      <c r="S59" t="s">
+        <v>70</v>
+      </c>
+      <c r="T59" t="s">
+        <v>70</v>
+      </c>
+      <c r="U59" t="s">
+        <v>70</v>
+      </c>
+      <c r="V59" t="s">
+        <v>70</v>
+      </c>
+      <c r="W59" t="s">
+        <v>70</v>
+      </c>
+      <c r="X59" t="s">
+        <v>70</v>
       </c>
       <c r="Y59" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="Z59">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA59" t="s">
         <v>79</v>
@@ -9286,28 +9351,28 @@
         <v>52</v>
       </c>
       <c r="AE59" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AF59" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="AG59" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="AH59" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="AI59">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AJ59" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
       <c r="AK59">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="AL59" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AM59" t="s">
         <v>60</v>
@@ -9325,90 +9390,90 @@
         <v>60</v>
       </c>
       <c r="AR59" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS59" t="s">
         <v>87</v>
       </c>
-      <c r="AS59" t="s">
-        <v>58</v>
-      </c>
       <c r="AT59" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AU59" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>151</v>
-      </c>
-      <c r="B60">
-        <v>1998</v>
+        <v>144</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
       </c>
       <c r="C60">
-        <v>42.55</v>
+        <v>37</v>
       </c>
       <c r="D60">
-        <v>0.36</v>
+        <v>0.47241149999999998</v>
       </c>
       <c r="E60" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F60" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G60">
         <v>6</v>
       </c>
       <c r="H60">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="I60">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J60">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K60">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L60">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="M60">
-        <v>-11.1</v>
+        <v>-10.6</v>
       </c>
       <c r="N60">
-        <v>9.76</v>
+        <v>8.6</v>
       </c>
       <c r="O60">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="P60">
         <v>18</v>
       </c>
       <c r="Q60">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R60">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="S60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T60">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="U60">
-        <v>-6.7</v>
+        <v>-7.6</v>
       </c>
       <c r="V60">
-        <v>9.61</v>
+        <v>7.5</v>
       </c>
       <c r="W60">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="X60">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="Y60" t="s">
         <v>48</v>
@@ -9429,7 +9494,7 @@
         <v>52</v>
       </c>
       <c r="AE60" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="AF60" t="s">
         <v>108</v>
@@ -9438,10 +9503,10 @@
         <v>80</v>
       </c>
       <c r="AH60" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="AI60">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AJ60" t="s">
         <v>48</v>
@@ -9474,78 +9539,78 @@
         <v>58</v>
       </c>
       <c r="AT60" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="AU60" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>152</v>
-      </c>
-      <c r="B61">
-        <v>2011</v>
-      </c>
-      <c r="C61">
-        <v>38.5</v>
-      </c>
-      <c r="D61">
-        <v>0.51133799999999996</v>
+        <v>145</v>
+      </c>
+      <c r="B61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" t="s">
+        <v>70</v>
       </c>
       <c r="E61" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F61" t="s">
-        <v>147</v>
-      </c>
-      <c r="G61">
+        <v>141</v>
+      </c>
+      <c r="G61" t="s">
+        <v>70</v>
+      </c>
+      <c r="H61">
+        <v>50</v>
+      </c>
+      <c r="I61">
+        <v>33</v>
+      </c>
+      <c r="J61">
+        <v>10</v>
+      </c>
+      <c r="K61" t="s">
+        <v>70</v>
+      </c>
+      <c r="L61" t="s">
+        <v>70</v>
+      </c>
+      <c r="M61" t="s">
+        <v>70</v>
+      </c>
+      <c r="N61" t="s">
+        <v>70</v>
+      </c>
+      <c r="O61" t="s">
+        <v>70</v>
+      </c>
+      <c r="P61" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q61">
+        <v>34</v>
+      </c>
+      <c r="R61">
         <v>8</v>
       </c>
-      <c r="H61">
-        <v>75</v>
-      </c>
-      <c r="I61">
-        <v>174</v>
-      </c>
-      <c r="J61">
-        <v>23</v>
-      </c>
-      <c r="K61">
-        <v>9</v>
-      </c>
-      <c r="L61">
-        <v>174</v>
-      </c>
-      <c r="M61">
-        <v>-10.76</v>
-      </c>
-      <c r="N61">
-        <v>6.6</v>
-      </c>
-      <c r="O61" t="s">
-        <v>70</v>
-      </c>
-      <c r="P61" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q61">
-        <v>184</v>
-      </c>
-      <c r="R61">
-        <v>17</v>
-      </c>
-      <c r="S61">
-        <v>2</v>
-      </c>
-      <c r="T61">
-        <v>184</v>
-      </c>
-      <c r="U61">
-        <v>-9.25</v>
-      </c>
-      <c r="V61">
-        <v>6.51</v>
+      <c r="S61" t="s">
+        <v>70</v>
+      </c>
+      <c r="T61" t="s">
+        <v>70</v>
+      </c>
+      <c r="U61" t="s">
+        <v>70</v>
+      </c>
+      <c r="V61" t="s">
+        <v>70</v>
       </c>
       <c r="W61" t="s">
         <v>70</v>
@@ -9557,10 +9622,10 @@
         <v>48</v>
       </c>
       <c r="Z61">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA61" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="AB61" t="s">
         <v>50</v>
@@ -9572,28 +9637,28 @@
         <v>52</v>
       </c>
       <c r="AE61" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AF61" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="AG61" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="AH61" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="AI61">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="AJ61" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="AK61">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AL61" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="AM61" t="s">
         <v>60</v>
@@ -9608,33 +9673,33 @@
         <v>59</v>
       </c>
       <c r="AQ61" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AR61" t="s">
         <v>60</v>
       </c>
       <c r="AS61" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="AT61" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="AU61" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>146</v>
-      </c>
-      <c r="B62" t="s">
-        <v>70</v>
+        <v>149</v>
+      </c>
+      <c r="B62">
+        <v>1998</v>
       </c>
       <c r="C62">
-        <v>38</v>
+        <v>41.75</v>
       </c>
       <c r="D62">
-        <v>0.6944999999999999</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="E62" t="s">
         <v>147</v>
@@ -9643,61 +9708,61 @@
         <v>147</v>
       </c>
       <c r="G62">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H62">
         <v>75</v>
       </c>
       <c r="I62">
-        <v>76</v>
-      </c>
-      <c r="J62">
+        <v>85</v>
+      </c>
+      <c r="J62" t="s">
+        <v>70</v>
+      </c>
+      <c r="K62">
+        <v>24</v>
+      </c>
+      <c r="L62">
+        <v>83</v>
+      </c>
+      <c r="M62">
+        <v>13.69</v>
+      </c>
+      <c r="N62">
+        <v>7.47</v>
+      </c>
+      <c r="O62">
+        <v>42</v>
+      </c>
+      <c r="P62">
         <v>19</v>
       </c>
-      <c r="K62">
-        <v>9</v>
-      </c>
-      <c r="L62">
-        <v>72</v>
-      </c>
-      <c r="M62">
-        <v>-10.92</v>
-      </c>
-      <c r="N62">
-        <v>6.63</v>
-      </c>
-      <c r="O62">
-        <v>28</v>
-      </c>
-      <c r="P62">
-        <v>11</v>
-      </c>
       <c r="Q62">
-        <v>79</v>
-      </c>
-      <c r="R62">
-        <v>25</v>
+        <v>95</v>
+      </c>
+      <c r="R62" t="s">
+        <v>70</v>
       </c>
       <c r="S62">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T62">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="U62">
-        <v>-9.49</v>
+        <v>17.25</v>
       </c>
       <c r="V62">
-        <v>8.1999999999999993</v>
+        <v>7.43</v>
       </c>
       <c r="W62">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="X62">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="Y62" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="Z62">
         <v>4</v>
@@ -9712,7 +9777,7 @@
         <v>51</v>
       </c>
       <c r="AD62" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="AE62" t="s">
         <v>71</v>
@@ -9724,19 +9789,19 @@
         <v>80</v>
       </c>
       <c r="AH62" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI62" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="AI62">
+        <v>20</v>
       </c>
       <c r="AJ62" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="AK62">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AL62" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="AM62" t="s">
         <v>60</v>
@@ -9754,13 +9819,13 @@
         <v>60</v>
       </c>
       <c r="AR62" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="AS62" t="s">
         <v>58</v>
       </c>
       <c r="AT62" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AU62" t="s">
         <v>62</v>
@@ -9768,16 +9833,16 @@
     </row>
     <row r="63" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>148</v>
-      </c>
-      <c r="B63" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63" t="s">
-        <v>70</v>
+        <v>151</v>
+      </c>
+      <c r="B63">
+        <v>1998</v>
+      </c>
+      <c r="C63">
+        <v>42.55</v>
       </c>
       <c r="D63">
-        <v>0.68500000000000005</v>
+        <v>0.36</v>
       </c>
       <c r="E63" t="s">
         <v>147</v>
@@ -9786,55 +9851,55 @@
         <v>147</v>
       </c>
       <c r="G63">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H63">
         <v>75</v>
       </c>
       <c r="I63">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="J63">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="K63">
+        <v>15</v>
+      </c>
+      <c r="L63">
+        <v>77</v>
+      </c>
+      <c r="M63">
+        <v>-11.1</v>
+      </c>
+      <c r="N63">
+        <v>9.76</v>
+      </c>
+      <c r="O63">
+        <v>33</v>
+      </c>
+      <c r="P63">
+        <v>18</v>
+      </c>
+      <c r="Q63">
+        <v>92</v>
+      </c>
+      <c r="R63">
+        <v>38</v>
+      </c>
+      <c r="S63">
         <v>5</v>
       </c>
-      <c r="L63">
-        <v>82</v>
-      </c>
-      <c r="M63">
-        <v>-15.59</v>
-      </c>
-      <c r="N63">
-        <v>10.72</v>
-      </c>
-      <c r="O63">
-        <v>48</v>
-      </c>
-      <c r="P63">
-        <v>32</v>
-      </c>
-      <c r="Q63">
-        <v>41.5</v>
-      </c>
-      <c r="R63">
-        <v>12</v>
-      </c>
-      <c r="S63">
-        <v>1.5</v>
-      </c>
       <c r="T63">
-        <v>40.5</v>
+        <v>92</v>
       </c>
       <c r="U63">
-        <v>-13.1</v>
+        <v>-6.7</v>
       </c>
       <c r="V63">
-        <v>10.63</v>
+        <v>9.61</v>
       </c>
       <c r="W63">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="X63">
         <v>12</v>
@@ -9846,7 +9911,7 @@
         <v>4</v>
       </c>
       <c r="AA63" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="AB63" t="s">
         <v>50</v>
@@ -9858,10 +9923,10 @@
         <v>52</v>
       </c>
       <c r="AE63" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AF63" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="AG63" t="s">
         <v>80</v>
@@ -9876,13 +9941,13 @@
         <v>48</v>
       </c>
       <c r="AK63">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AL63" t="s">
         <v>48</v>
       </c>
       <c r="AM63" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AN63" t="s">
         <v>60</v>
@@ -9903,159 +9968,598 @@
         <v>58</v>
       </c>
       <c r="AT63" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64">
+        <v>2011</v>
+      </c>
+      <c r="C64">
+        <v>38.5</v>
+      </c>
+      <c r="D64">
+        <v>0.51133799999999996</v>
+      </c>
+      <c r="E64" t="s">
+        <v>147</v>
+      </c>
+      <c r="F64" t="s">
+        <v>147</v>
+      </c>
+      <c r="G64">
+        <v>8</v>
+      </c>
+      <c r="H64">
+        <v>75</v>
+      </c>
+      <c r="I64">
+        <v>174</v>
+      </c>
+      <c r="J64">
+        <v>23</v>
+      </c>
+      <c r="K64">
+        <v>9</v>
+      </c>
+      <c r="L64">
+        <v>174</v>
+      </c>
+      <c r="M64">
+        <v>-10.76</v>
+      </c>
+      <c r="N64">
+        <v>6.6</v>
+      </c>
+      <c r="O64" t="s">
+        <v>70</v>
+      </c>
+      <c r="P64" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q64">
+        <v>184</v>
+      </c>
+      <c r="R64">
+        <v>17</v>
+      </c>
+      <c r="S64">
+        <v>2</v>
+      </c>
+      <c r="T64">
+        <v>184</v>
+      </c>
+      <c r="U64">
+        <v>-9.25</v>
+      </c>
+      <c r="V64">
+        <v>6.51</v>
+      </c>
+      <c r="W64" t="s">
+        <v>70</v>
+      </c>
+      <c r="X64" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z64">
+        <v>3</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC64" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD64" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE64" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF64" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG64" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH64" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI64">
+        <v>26</v>
+      </c>
+      <c r="AJ64" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK64">
+        <v>8</v>
+      </c>
+      <c r="AL64" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM64" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN64" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO64" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP64" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ64" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR64" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS64" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT64" t="s">
+        <v>66</v>
+      </c>
+      <c r="AU64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>146</v>
+      </c>
+      <c r="B65" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65">
+        <v>38</v>
+      </c>
+      <c r="D65">
+        <v>0.6944999999999999</v>
+      </c>
+      <c r="E65" t="s">
+        <v>147</v>
+      </c>
+      <c r="F65" t="s">
+        <v>147</v>
+      </c>
+      <c r="G65">
+        <v>6</v>
+      </c>
+      <c r="H65">
+        <v>75</v>
+      </c>
+      <c r="I65">
+        <v>76</v>
+      </c>
+      <c r="J65">
+        <v>19</v>
+      </c>
+      <c r="K65">
+        <v>9</v>
+      </c>
+      <c r="L65">
+        <v>72</v>
+      </c>
+      <c r="M65">
+        <v>-10.92</v>
+      </c>
+      <c r="N65">
+        <v>6.63</v>
+      </c>
+      <c r="O65">
+        <v>28</v>
+      </c>
+      <c r="P65">
+        <v>11</v>
+      </c>
+      <c r="Q65">
+        <v>79</v>
+      </c>
+      <c r="R65">
+        <v>25</v>
+      </c>
+      <c r="S65">
+        <v>5</v>
+      </c>
+      <c r="T65">
+        <v>75</v>
+      </c>
+      <c r="U65">
+        <v>-9.49</v>
+      </c>
+      <c r="V65">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="W65">
+        <v>26</v>
+      </c>
+      <c r="X65">
+        <v>13</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z65">
+        <v>4</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC65" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD65" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE65" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF65" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG65" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH65" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI65" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ65" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK65">
+        <v>6</v>
+      </c>
+      <c r="AL65" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM65" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN65" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO65" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP65" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ65" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR65" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS65" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT65" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>148</v>
+      </c>
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="E66" t="s">
+        <v>147</v>
+      </c>
+      <c r="F66" t="s">
+        <v>147</v>
+      </c>
+      <c r="G66">
+        <v>8</v>
+      </c>
+      <c r="H66">
+        <v>75</v>
+      </c>
+      <c r="I66">
+        <v>83</v>
+      </c>
+      <c r="J66">
+        <v>17</v>
+      </c>
+      <c r="K66">
+        <v>5</v>
+      </c>
+      <c r="L66">
+        <v>82</v>
+      </c>
+      <c r="M66">
+        <v>-15.59</v>
+      </c>
+      <c r="N66">
+        <v>10.72</v>
+      </c>
+      <c r="O66">
+        <v>48</v>
+      </c>
+      <c r="P66">
+        <v>32</v>
+      </c>
+      <c r="Q66">
+        <v>41.5</v>
+      </c>
+      <c r="R66">
+        <v>12</v>
+      </c>
+      <c r="S66">
+        <v>1.5</v>
+      </c>
+      <c r="T66">
+        <v>40.5</v>
+      </c>
+      <c r="U66">
+        <v>-13.1</v>
+      </c>
+      <c r="V66">
+        <v>10.63</v>
+      </c>
+      <c r="W66">
+        <v>20</v>
+      </c>
+      <c r="X66">
+        <v>12</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z66">
+        <v>4</v>
+      </c>
+      <c r="AA66" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC66" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD66" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE66" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF66" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG66" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH66" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI66">
+        <v>20</v>
+      </c>
+      <c r="AJ66" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK66">
+        <v>8</v>
+      </c>
+      <c r="AL66" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM66" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN66" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO66" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP66" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ66" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR66" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS66" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT66" t="s">
         <v>61</v>
       </c>
-      <c r="AU63" t="s">
+      <c r="AU66" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
+    <row r="67" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B67" s="2">
         <v>2000</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C67" s="2">
         <v>40.519999999999996</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E64" s="2" t="s">
+      <c r="D67" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G67" s="2">
         <v>8</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H67" s="2">
         <v>20</v>
       </c>
-      <c r="I64" s="2">
+      <c r="I67" s="2">
         <v>33</v>
       </c>
-      <c r="J64" s="2">
+      <c r="J67" s="2">
         <v>12</v>
       </c>
-      <c r="K64" s="2">
+      <c r="K67" s="2">
         <v>1</v>
       </c>
-      <c r="L64" s="2">
+      <c r="L67" s="2">
         <v>33</v>
       </c>
-      <c r="M64" s="2">
+      <c r="M67" s="2">
         <v>-7.75</v>
       </c>
-      <c r="N64" s="2">
+      <c r="N67" s="2">
         <v>6.89</v>
       </c>
-      <c r="O64" s="2">
+      <c r="O67" s="2">
         <v>15</v>
       </c>
-      <c r="P64" s="2">
+      <c r="P67" s="2">
         <v>33</v>
       </c>
-      <c r="Q64" s="2">
-        <v>70</v>
-      </c>
-      <c r="R64" s="2">
+      <c r="Q67" s="2">
+        <v>70</v>
+      </c>
+      <c r="R67" s="2">
         <v>24</v>
       </c>
-      <c r="S64" s="2">
+      <c r="S67" s="2">
         <v>3</v>
       </c>
-      <c r="T64" s="2">
+      <c r="T67" s="2">
         <v>66</v>
       </c>
-      <c r="U64" s="2">
+      <c r="U67" s="2">
         <v>-6.61</v>
       </c>
-      <c r="V64" s="2">
+      <c r="V67" s="2">
         <v>6.74</v>
       </c>
-      <c r="W64" s="2">
+      <c r="W67" s="2">
         <v>24</v>
       </c>
-      <c r="X64" s="2">
+      <c r="X67" s="2">
         <v>66</v>
       </c>
-      <c r="Y64" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z64" s="2">
+      <c r="Y67" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z67" s="2">
         <v>3</v>
       </c>
-      <c r="AA64" s="2" t="s">
+      <c r="AA67" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AB64" s="2" t="s">
+      <c r="AB67" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AC64" s="2" t="s">
+      <c r="AC67" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AD64" s="2" t="s">
+      <c r="AD67" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AE64" s="2" t="s">
+      <c r="AE67" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AF64" s="2" t="s">
+      <c r="AF67" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AG64" s="2" t="s">
+      <c r="AG67" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AH64" s="2" t="s">
+      <c r="AH67" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AI64" s="2">
+      <c r="AI67" s="2">
         <v>15</v>
       </c>
-      <c r="AJ64" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AK64" s="2">
+      <c r="AJ67" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK67" s="2">
         <v>10</v>
       </c>
-      <c r="AL64" s="2" t="s">
+      <c r="AL67" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AM64" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN64" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO64" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP64" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ64" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AR64" s="2" t="s">
+      <c r="AM67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO67" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP67" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR67" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AS64" s="2" t="s">
+      <c r="AS67" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AT64" s="2" t="s">
+      <c r="AT67" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AU64" s="2" t="s">
+      <c r="AU67" s="2" t="s">
         <v>62</v>
       </c>
+    </row>
+    <row r="68" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
+      <c r="X68" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AV125">
-    <sortCondition ref="G2:G125"/>
-    <sortCondition ref="B2:B125"/>
+  <sortState ref="A2:AV128">
+    <sortCondition ref="G2:G128"/>
+    <sortCondition ref="B2:B128"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>